<commit_message>
nMDS index reversals and phenomix buildout; long-term trend plots
</commit_message>
<xml_diff>
--- a/Biol_files_2025/CopeSppGroupingsand_ListOfNames_Peterson_etal_2011.xlsx
+++ b/Biol_files_2025/CopeSppGroupingsand_ListOfNames_Peterson_etal_2011.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Documents\Coding\Project_Repositories\Lilly_etal_XX_NCC_CopepodBSTPhysDrivers_v2\Biol_files_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EB01A48-1370-4C00-841C-C643887A1194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CED131-93C5-4B36-8183-842CBC7E9D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Summary_of_CopeGroups" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -444,9 +443,6 @@
     <t>Calocalanus styliremis</t>
   </si>
   <si>
-    <t>Calocalanus tenuis</t>
-  </si>
-  <si>
     <t>Clausocalanus spp.</t>
   </si>
   <si>
@@ -456,9 +452,6 @@
     <t>Ctenocalanus vanus</t>
   </si>
   <si>
-    <t>Mesocalanus tenuicornis</t>
-  </si>
-  <si>
     <t>Paracalanus parvus</t>
   </si>
   <si>
@@ -466,6 +459,12 @@
   </si>
   <si>
     <t>Clausocalanus spp. --&gt; All to sum</t>
+  </si>
+  <si>
+    <t>Calocalanus tenuis (CALTENU)</t>
+  </si>
+  <si>
+    <t>Mesocalanus tenuicornis (CALTEN)</t>
   </si>
 </sst>
 </file>
@@ -4997,13 +4996,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCFF003-0CF7-47E6-8F6A-93FACE9F4ADC}">
   <dimension ref="A3:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
     <col min="2" max="2" width="3.90625" customWidth="1"/>
     <col min="3" max="3" width="21.7265625" customWidth="1"/>
   </cols>
@@ -5030,7 +5029,7 @@
         <v>136</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -5057,7 +5056,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
         <v>36</v>
@@ -5065,7 +5064,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" t="s">
         <v>96</v>
@@ -5073,7 +5072,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" t="s">
         <v>113</v>
@@ -5081,7 +5080,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F12" t="s">
         <v>37</v>
@@ -5089,7 +5088,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -5097,7 +5096,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F14" t="s">
         <v>85</v>
@@ -5105,7 +5104,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>

</xml_diff>